<commit_message>
feat(FN-1945): change fees paid report header
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DD4C435-1D4C-4806-98AD-4E7834AA7CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BB1FF7-3916-418B-A6F5-3B5656C3FC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
   </bookViews>
   <sheets>
     <sheet name="invalid-utilisation-report" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Total fees accrued for the month</t>
   </si>
   <si>
-    <t>Monthly fees paid to UKEF</t>
-  </si>
-  <si>
     <t>GBP</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Potato Exporter</t>
+  </si>
+  <si>
+    <t>Fees paid to UKEF for the period</t>
   </si>
 </sst>
 </file>
@@ -199,9 +199,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -239,7 +239,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -345,7 +345,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -498,19 +498,19 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,21 +533,21 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4">
         <v>20001371123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="6">
         <v>600000</v>
@@ -560,18 +560,18 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="6">
         <v>300000</v>
@@ -582,18 +582,18 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>20001499</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6">
         <v>1500000</v>
@@ -608,18 +608,18 @@
         <v>976.23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>20001507</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6">
         <v>2500000</v>

</xml_diff>

<commit_message>
feat(FN-1945): change fees paid report header (#2560)
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DD4C435-1D4C-4806-98AD-4E7834AA7CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BB1FF7-3916-418B-A6F5-3B5656C3FC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
   </bookViews>
   <sheets>
     <sheet name="invalid-utilisation-report" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Total fees accrued for the month</t>
   </si>
   <si>
-    <t>Monthly fees paid to UKEF</t>
-  </si>
-  <si>
     <t>GBP</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Potato Exporter</t>
+  </si>
+  <si>
+    <t>Fees paid to UKEF for the period</t>
   </si>
 </sst>
 </file>
@@ -199,9 +199,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -239,7 +239,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -345,7 +345,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -498,19 +498,19 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,21 +533,21 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4">
         <v>20001371123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="6">
         <v>600000</v>
@@ -560,18 +560,18 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="6">
         <v>300000</v>
@@ -582,18 +582,18 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>20001499</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6">
         <v>1500000</v>
@@ -608,18 +608,18 @@
         <v>976.23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
         <v>20001507</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6">
         <v>2500000</v>

</xml_diff>

<commit_message>
feat(FN-2022): update e2e fixtures
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BB1FF7-3916-418B-A6F5-3B5656C3FC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AE07A6-2611-4785-9B7D-EB9E74056813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Facility utilisatin</t>
   </si>
   <si>
-    <t>Total fees accrued for the month</t>
-  </si>
-  <si>
     <t>GBP</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Fees paid to UKEF for the period</t>
+  </si>
+  <si>
+    <t>Fees accrued since last report</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,24 +530,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4">
         <v>20001371123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6">
         <v>600000</v>
@@ -562,16 +562,16 @@
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="6">
         <v>300000</v>
@@ -584,16 +584,16 @@
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>20001499</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6">
         <v>1500000</v>
@@ -610,16 +610,16 @@
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4">
         <v>20001507</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6">
         <v>2500000</v>

</xml_diff>

<commit_message>
feat(FN-2022): update name again
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AE07A6-2611-4785-9B7D-EB9E74056813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D343A754-AAA3-4F3E-AD83-DD55D43B1182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
   </bookViews>
@@ -98,7 +98,7 @@
     <t>Fees paid to UKEF for the period</t>
   </si>
   <si>
-    <t>Fees accrued since last report</t>
+    <t>Total fees accrued for the period</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat(FN-2022): update total fees report header (#2580)
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josbin\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BB1FF7-3916-418B-A6F5-3B5656C3FC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D343A754-AAA3-4F3E-AD83-DD55D43B1182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9AB75A7F-EBE7-4889-9C82-832E0A4F8807}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Facility utilisatin</t>
   </si>
   <si>
-    <t>Total fees accrued for the month</t>
-  </si>
-  <si>
     <t>GBP</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Fees paid to UKEF for the period</t>
+  </si>
+  <si>
+    <t>Total fees accrued for the period</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,24 +530,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4">
         <v>20001371123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6">
         <v>600000</v>
@@ -562,16 +562,16 @@
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="6">
         <v>300000</v>
@@ -584,16 +584,16 @@
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>20001499</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6">
         <v>1500000</v>
@@ -610,16 +610,16 @@
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4">
         <v>20001507</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6">
         <v>2500000</v>

</xml_diff>